<commit_message>
Excel Order template name issue-fixed
Excel Order template name issue-fixed
</commit_message>
<xml_diff>
--- a/public/template/Flower_sample_template.xlsx
+++ b/public/template/Flower_sample_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tester\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30177378-9BCF-4FA0-AD6F-C74826A8EB83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F8E5C0F-05EA-4BC2-96D4-B5C1B7DC5738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t>Order Received Data and Time</t>
   </si>
@@ -110,12 +110,6 @@
     <t>Baldwin</t>
   </si>
   <si>
-    <t>Typist</t>
-  </si>
-  <si>
-    <t>Typist QC</t>
-  </si>
-  <si>
     <t>FTC18-001</t>
   </si>
   <si>
@@ -126,6 +120,9 @@
   </si>
   <si>
     <t>Policy Typing</t>
+  </si>
+  <si>
+    <t>Production &amp; QC</t>
   </si>
 </sst>
 </file>
@@ -1019,26 +1016,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="A4" sqref="A4:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1"/>
-    <col min="7" max="7" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="34.5546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.77734375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.77734375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1052,45 +1050,39 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="O1" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>45509.0625</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>11</v>
@@ -1099,41 +1091,37 @@
         <v>12</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1" t="s">
+      <c r="K2" s="1"/>
+      <c r="L2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>45510.0625</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>16</v>
@@ -1141,39 +1129,34 @@
       <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="G3" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="J3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1" t="s">
+      <c r="K3" s="1"/>
+      <c r="L3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="E3">
-    <cfRule type="uniqueValues" dxfId="0" priority="1"/>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>